<commit_message>
All changes on March 4, 2017
- New stl files,
- iPhone remote created.
- Some Arduino test code added.
</commit_message>
<xml_diff>
--- a/Robotics.xlsx
+++ b/Robotics.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Neil/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Neil/Desktop/Robotics Quadcopter Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="460" windowWidth="25480" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="120" yWindow="460" windowWidth="25480" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
   <si>
     <t>Todos</t>
   </si>
@@ -129,9 +129,6 @@
     <t xml:space="preserve">Begin to reflect upon the project and schedule. </t>
   </si>
   <si>
-    <t>If time allows, do person tracking</t>
-  </si>
-  <si>
     <t>Project writeup</t>
   </si>
   <si>
@@ -145,13 +142,50 @@
   </si>
   <si>
     <t>Develop PID</t>
+  </si>
+  <si>
+    <t>Implement GPS hardware</t>
+  </si>
+  <si>
+    <t>Develop software for GPS</t>
+  </si>
+  <si>
+    <t>Test final product</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Kootek-MPU-6050-MPU6050-sensors-Accelerometer/dp/B008BOPN40/ref=sr_1_4?ie=UTF8&amp;qid=1488655663&amp;sr=8-4&amp;keywords=mpu+6050</t>
+  </si>
+  <si>
+    <t>Wood Screw 34mm, 19mm, 12mm * 3mm 6g A2 Stainless Steel</t>
+  </si>
+  <si>
+    <t>http://www.ebay.com/itm/3mm-6g-A2-STAINLESS-STEEL-WOOD-SCREWS-POZI-CSK-10mm-THROUGH-TO-50mm-/190718538596?var=&amp;hash=item2c67b5f364:m:mWmH-3MwpEqMHxtEfEkZxsw</t>
+  </si>
+  <si>
+    <t>Folding props</t>
+  </si>
+  <si>
+    <t>http://www.ebay.com/itm/4x-DJI-Mavic-Pro-Quadcopter-Drone-8330-Quick-Release-Folding-Propellers-Black-/122276747402?hash=item1c7843188a:g:kl4AAOSwZQRYWIr5</t>
+  </si>
+  <si>
+    <t>SD Card writer</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Storage-Shield-Module-Interface-Arduino/dp/B00SL0QWDU/ref=sr_1_2?ie=UTF8&amp;qid=1488682723&amp;sr=8-2&amp;keywords=Arduino+sd+card</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -186,21 +220,40 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF111111"/>
-      <name val="Times Roman"/>
+      <name val="Times New Roman"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Times New Roman"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -212,22 +265,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="14" fontId="6" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="6" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="20% - Accent3" xfId="2" builtinId="38"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -270,7 +330,7 @@
           <c:x val="0.0174825174825175"/>
           <c:y val="0.0197044334975369"/>
           <c:w val="0.95979020979021"/>
-          <c:h val="0.926108374384236"/>
+          <c:h val="0.945381049213166"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -280,9 +340,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>Start Data</c:v>
-          </c:tx>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -293,9 +350,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$13</c:f>
+              <c:f>Sheet1!$A$2:$A$14</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>Design the frame</c:v>
                 </c:pt>
@@ -327,55 +384,64 @@
                   <c:v>Begin to reflect upon the project and schedule. </c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>If time allows, do person tracking</c:v>
+                  <c:v>Implement GPS hardware</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Project writeup</c:v>
+                  <c:v>Develop software for GPS</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Test final product</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$13</c:f>
+              <c:f>Sheet1!$B$2:$B$15</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>42804.0</c:v>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>42814.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42827.0</c:v>
+                  <c:v>42822.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42830.0</c:v>
+                  <c:v>42823.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>42826.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>42833.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>42835.0</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>42845.0</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>42848.0</c:v>
+                  <c:v>42843.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>42853.0</c:v>
+                  <c:v>42850.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>42855.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>42856.0</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>42862.0</c:v>
-                </c:pt>
                 <c:pt idx="10">
-                  <c:v>42864.0</c:v>
+                  <c:v>42860.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>42864.0</c:v>
+                  <c:v>42863.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42874.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42856.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -384,9 +450,6 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>Duration</c:v>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent2"/>
@@ -399,9 +462,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$13</c:f>
+              <c:f>Sheet1!$A$2:$A$14</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>Design the frame</c:v>
                 </c:pt>
@@ -433,55 +496,64 @@
                   <c:v>Begin to reflect upon the project and schedule. </c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>If time allows, do person tracking</c:v>
+                  <c:v>Implement GPS hardware</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Project writeup</c:v>
+                  <c:v>Develop software for GPS</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Test final product</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$13</c:f>
+              <c:f>Sheet1!$C$2:$C$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>23.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>5.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>14.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>20.0</c:v>
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>25.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -497,11 +569,11 @@
         </c:dLbls>
         <c:gapWidth val="30"/>
         <c:overlap val="100"/>
-        <c:axId val="-775910032"/>
-        <c:axId val="-775908256"/>
+        <c:axId val="344521296"/>
+        <c:axId val="344523344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-775910032"/>
+        <c:axId val="344521296"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -511,7 +583,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-775908256"/>
+        <c:crossAx val="344523344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -519,18 +591,19 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-775908256"/>
+        <c:axId val="344523344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="42885.0"/>
-          <c:min val="42804.0"/>
+          <c:min val="42814.0"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="t"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-775910032"/>
+        <c:crossAx val="344521296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1121,16 +1194,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>673100</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>18814</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:rowOff>136878</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>138684</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>103482</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1417,232 +1490,258 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView zoomScale="135" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="10.5" style="5" customWidth="1"/>
-    <col min="4" max="9" width="10.83203125" style="5"/>
-    <col min="11" max="12" width="10.83203125" style="5"/>
-    <col min="13" max="13" width="13" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="10.83203125" style="5"/>
+    <col min="1" max="1" width="17.83203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="10.5" style="4" customWidth="1"/>
+    <col min="4" max="4" width="13" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="5" t="s">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="6">
+        <v>42814</v>
+      </c>
+      <c r="C2" s="4">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6">
+        <v>42821</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="6">
+        <v>42822</v>
+      </c>
+      <c r="C3" s="4">
+        <v>5</v>
+      </c>
+      <c r="D3" s="6">
+        <v>42827</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="6">
+        <v>42823</v>
+      </c>
+      <c r="C4" s="4">
+        <v>5</v>
+      </c>
+      <c r="D4" s="6">
+        <v>42829</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="6">
+        <v>42826</v>
+      </c>
+      <c r="C5" s="4">
+        <v>7</v>
+      </c>
+      <c r="D5" s="6">
+        <v>42832</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A6" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K1" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="M1" s="5" t="s">
+      <c r="B6" s="6">
+        <v>42833</v>
+      </c>
+      <c r="C6" s="4">
+        <v>7</v>
+      </c>
+      <c r="D6" s="6">
+        <v>42840</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="6">
+        <v>42835</v>
+      </c>
+      <c r="C7" s="4">
+        <v>8</v>
+      </c>
+      <c r="D7" s="6">
+        <v>42842</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="6">
+        <v>42843</v>
+      </c>
+      <c r="C8" s="4">
+        <v>7</v>
+      </c>
+      <c r="D8" s="6">
+        <v>42850</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="6">
+        <v>42850</v>
+      </c>
+      <c r="C9" s="4">
+        <v>5</v>
+      </c>
+      <c r="D9" s="6">
+        <v>42855</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="6">
+        <v>42855</v>
+      </c>
+      <c r="C10" s="4">
+        <v>5</v>
+      </c>
+      <c r="D10" s="6">
+        <v>42859</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="6">
+        <v>42856</v>
+      </c>
+      <c r="C11" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="D11" s="6">
+        <v>42859</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="13">
+        <v>42860</v>
+      </c>
+      <c r="C12" s="12">
+        <v>4</v>
+      </c>
+      <c r="D12" s="13">
+        <v>42862</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="11">
+        <v>42863</v>
+      </c>
+      <c r="C13" s="10">
+        <v>10</v>
+      </c>
+      <c r="D13" s="11">
+        <v>42873</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="11">
+        <v>42874</v>
+      </c>
+      <c r="C14" s="10">
+        <v>7</v>
+      </c>
+      <c r="D14" s="11">
+        <v>42880</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="6">
+        <v>42856</v>
+      </c>
+      <c r="C15" s="4">
         <v>25</v>
       </c>
-      <c r="B2" s="8">
-        <v>42804</v>
-      </c>
-      <c r="C2" s="5">
-        <v>23</v>
-      </c>
-      <c r="M2" s="7">
-        <v>42826</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="7">
-        <v>42827</v>
-      </c>
-      <c r="C3" s="5">
-        <v>3</v>
-      </c>
-      <c r="M3" s="7">
-        <v>42829</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="7">
-        <v>42830</v>
-      </c>
-      <c r="C4" s="5">
-        <v>3</v>
-      </c>
-      <c r="M4" s="7">
-        <v>42832</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="7">
-        <v>42833</v>
-      </c>
-      <c r="C5" s="5">
-        <v>5</v>
-      </c>
-      <c r="M5" s="7">
-        <v>42837</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="7">
-        <v>42835</v>
-      </c>
-      <c r="C6" s="5">
-        <v>10</v>
-      </c>
-      <c r="M6" s="7">
-        <v>42844</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="7">
-        <v>42845</v>
-      </c>
-      <c r="C7" s="5">
-        <v>3</v>
-      </c>
-      <c r="M7" s="7">
-        <v>42847</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="7">
-        <v>42848</v>
-      </c>
-      <c r="C8" s="5">
-        <v>5</v>
-      </c>
-      <c r="M8" s="7">
-        <v>42852</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="7">
-        <v>42853</v>
-      </c>
-      <c r="C9" s="5">
-        <v>3</v>
-      </c>
-      <c r="M9" s="7">
-        <v>42855</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="7">
-        <v>42856</v>
-      </c>
-      <c r="C10" s="5">
-        <v>7</v>
-      </c>
-      <c r="M10" s="7">
-        <v>42861</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="7">
-        <v>42862</v>
-      </c>
-      <c r="C11" s="5">
-        <v>3</v>
-      </c>
-      <c r="M11" s="7">
-        <v>42863</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="7">
-        <v>42864</v>
-      </c>
-      <c r="C12" s="5">
-        <v>14</v>
-      </c>
-      <c r="M12" s="7">
-        <v>42877</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="7">
-        <v>42864</v>
-      </c>
-      <c r="C13" s="5">
-        <v>20</v>
-      </c>
-      <c r="M13" s="7">
-        <v>42886</v>
-      </c>
-    </row>
-    <row r="17" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M17" s="6"/>
+      <c r="D15" s="6">
+        <v>42875</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="D17" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1653,209 +1752,284 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" style="9" customWidth="1"/>
+    <col min="2" max="3" width="10.83203125" style="9"/>
+    <col min="4" max="4" width="13" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="4">
         <v>38.33</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="4">
         <v>1</v>
       </c>
-      <c r="D2" s="1">
-        <f t="shared" ref="D2:D6" si="0">B2*C2</f>
+      <c r="D2" s="4">
+        <f t="shared" ref="D2:D7" si="0">B2*C2</f>
         <v>38.33</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="4">
         <v>13.99</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="4">
         <v>1</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="4">
         <f t="shared" si="0"/>
         <v>13.99</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="4">
         <v>19.95</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="4">
         <v>1</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="4">
         <f t="shared" si="0"/>
         <v>19.95</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="4">
+        <v>17.66</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4">
+        <f>B5*C5</f>
+        <v>17.66</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="1">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="C5" s="1">
+      <c r="B6" s="4">
+        <v>6.94</v>
+      </c>
+      <c r="C6" s="4">
         <v>0</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D6" s="4">
+        <f>B6*C6</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="4">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="1">
-        <v>9.9499999999999993</v>
-      </c>
-      <c r="C6" s="1">
+      <c r="E7" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C8" s="4">
         <v>0</v>
       </c>
-      <c r="D6" s="1">
-        <f t="shared" si="0"/>
+      <c r="D8" s="4">
+        <f>B8*C8</f>
         <v>0</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1">
-        <f>D6+D4+D5+D3+D2</f>
-        <v>72.27</v>
-      </c>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="E8" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4">
+        <f>D7+D4+D6+D3+D2+D5</f>
+        <v>89.929999999999993</v>
+      </c>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11">
-        <v>58</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <f>B11*C11</f>
-        <v>58</v>
-      </c>
-      <c r="E11" t="s">
-        <v>19</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="1">
-        <v>17.66</v>
-      </c>
-      <c r="C12" s="1">
+        <v>18</v>
+      </c>
+      <c r="B12" s="4">
+        <v>58</v>
+      </c>
+      <c r="C12" s="4">
         <v>1</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="4">
         <f>B12*C12</f>
-        <v>17.66</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>14</v>
+        <v>58</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1">
-        <v>12.95</v>
+        <v>17.66</v>
       </c>
       <c r="C13" s="1">
         <v>1</v>
       </c>
       <c r="D13" s="1">
         <f>B13*C13</f>
+        <v>17.66</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="1">
         <v>12.95</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
+        <f>B14*C14</f>
+        <v>12.95</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="4">
+        <v>16.28</v>
+      </c>
+      <c r="C15" s="4">
+        <v>1</v>
+      </c>
+      <c r="D15" s="4">
+        <f>B15*C15</f>
+        <v>16.28</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A16" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="4">
+        <v>5.9</v>
+      </c>
+      <c r="C16" s="4">
+        <v>1</v>
+      </c>
+      <c r="D16" s="4">
+        <f>B16*C16</f>
+        <v>5.9</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E13" r:id="rId1"/>
+    <hyperlink ref="E14" r:id="rId1"/>
     <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="E8" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
All changes on March 5
- iPhone controller UI finished.
- Gcode added.
- Parts list and proposal updated.
- Other small changes.
</commit_message>
<xml_diff>
--- a/Robotics.xlsx
+++ b/Robotics.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
   <si>
     <t>Todos</t>
   </si>
@@ -120,12 +120,6 @@
     <t>Test leveling and movement</t>
   </si>
   <si>
-    <t>Finish Bluetooth</t>
-  </si>
-  <si>
-    <t>Final testing for bluetooth, self-balancing</t>
-  </si>
-  <si>
     <t xml:space="preserve">Begin to reflect upon the project and schedule. </t>
   </si>
   <si>
@@ -172,13 +166,28 @@
   </si>
   <si>
     <t>https://www.amazon.com/Storage-Shield-Module-Interface-Arduino/dp/B00SL0QWDU/ref=sr_1_2?ie=UTF8&amp;qid=1488682723&amp;sr=8-2&amp;keywords=Arduino+sd+card</t>
+  </si>
+  <si>
+    <t>Radio Transmitter &amp; Reciever</t>
+  </si>
+  <si>
+    <t>http://www.ebay.com/itm/New-Flysky-2-4G-FS-T4B-4-CH-Channel-Radio-Control-RC-Transmitter-Receiver-X9M8-/291899124014?hash=item43f68b292e:g:7hYAAOSw8gVX8ywU</t>
+  </si>
+  <si>
+    <t>Develop iOS Application</t>
+  </si>
+  <si>
+    <t>Develop Wireless controlling</t>
+  </si>
+  <si>
+    <t>Test wireless control</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -241,6 +250,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -265,10 +282,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -286,8 +311,16 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="6" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="11">
     <cellStyle name="20% - Accent3" xfId="2" builtinId="38"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -327,10 +360,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0174825174825175"/>
-          <c:y val="0.0197044334975369"/>
-          <c:w val="0.95979020979021"/>
-          <c:h val="0.945381049213166"/>
+          <c:x val="0.00722942178754074"/>
+          <c:y val="0.0145607041629438"/>
+          <c:w val="0.968334545906653"/>
+          <c:h val="0.955668629965322"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -360,25 +393,25 @@
                   <c:v>Print frame</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Develop iOS Application</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Assemble frame</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Electronics</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>Develop Wireless controlling</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Test wireless control</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>Develop PID</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>Test leveling and movement</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Finish Bluetooth</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Test leveling and movement</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Final testing for bluetooth, self-balancing</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Begin to reflect upon the project and schedule. </c:v>
@@ -408,34 +441,34 @@
                   <c:v>42822.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42823.0</c:v>
+                  <c:v>42822.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42826.0</c:v>
+                  <c:v>42824.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42833.0</c:v>
+                  <c:v>42829.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>42835.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42843.0</c:v>
+                  <c:v>42841.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>42850.0</c:v>
+                  <c:v>42844.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>42855.0</c:v>
+                  <c:v>42849.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>42854.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>42856.0</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>42860.0</c:v>
-                </c:pt>
                 <c:pt idx="11">
-                  <c:v>42863.0</c:v>
+                  <c:v>42861.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>42874.0</c:v>
@@ -472,25 +505,25 @@
                   <c:v>Print frame</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Develop iOS Application</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Assemble frame</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Electronics</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>Develop Wireless controlling</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Test wireless control</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>Develop PID</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>Test leveling and movement</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Finish Bluetooth</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Test leveling and movement</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Final testing for bluetooth, self-balancing</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Begin to reflect upon the project and schedule. </c:v>
@@ -520,22 +553,22 @@
                   <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.0</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>5.0</c:v>
@@ -544,10 +577,10 @@
                   <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.0</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10.0</c:v>
+                  <c:v>14.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>7.0</c:v>
@@ -569,11 +602,11 @@
         </c:dLbls>
         <c:gapWidth val="30"/>
         <c:overlap val="100"/>
-        <c:axId val="344521296"/>
-        <c:axId val="344523344"/>
+        <c:axId val="695017184"/>
+        <c:axId val="695031600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="344521296"/>
+        <c:axId val="695017184"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -583,7 +616,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="344523344"/>
+        <c:crossAx val="695031600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -591,7 +624,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="344523344"/>
+        <c:axId val="695031600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="42885.0"/>
@@ -603,7 +636,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="344521296"/>
+        <c:crossAx val="695017184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1490,8 +1523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView zoomScale="135" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView zoomScale="140" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1517,31 +1550,31 @@
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.15">
@@ -1569,113 +1602,113 @@
         <v>5</v>
       </c>
       <c r="D3" s="6">
-        <v>42827</v>
+        <v>42796</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="B4" s="6">
-        <v>42823</v>
+        <v>42822</v>
       </c>
       <c r="C4" s="4">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D4" s="6">
-        <v>42829</v>
+        <v>42832</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B5" s="6">
-        <v>42826</v>
+        <v>42824</v>
       </c>
       <c r="C5" s="4">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D5" s="6">
-        <v>42832</v>
+        <v>42829</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B6" s="6">
-        <v>42833</v>
+        <v>42829</v>
       </c>
       <c r="C6" s="4">
         <v>7</v>
       </c>
       <c r="D6" s="6">
-        <v>42840</v>
+        <v>42832</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="B7" s="6">
         <v>42835</v>
       </c>
       <c r="C7" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" s="6">
-        <v>42842</v>
+        <v>42841</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="B8" s="6">
-        <v>42843</v>
+        <v>42841</v>
       </c>
       <c r="C8" s="4">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D8" s="6">
-        <v>42850</v>
+        <v>42844</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B9" s="6">
-        <v>42850</v>
+        <v>42844</v>
       </c>
       <c r="C9" s="4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D9" s="6">
-        <v>42855</v>
+        <v>42848</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B10" s="6">
-        <v>42855</v>
+        <v>42849</v>
       </c>
       <c r="C10" s="4">
         <v>5</v>
       </c>
       <c r="D10" s="6">
-        <v>42859</v>
+        <v>42853</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B11" s="6">
-        <v>42856</v>
+        <v>42854</v>
       </c>
       <c r="C11" s="4">
         <v>3</v>
@@ -1686,27 +1719,27 @@
     </row>
     <row r="12" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A12" s="12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B12" s="13">
+        <v>42856</v>
+      </c>
+      <c r="C12" s="12">
+        <v>5</v>
+      </c>
+      <c r="D12" s="13">
         <v>42860</v>
-      </c>
-      <c r="C12" s="12">
-        <v>4</v>
-      </c>
-      <c r="D12" s="13">
-        <v>42862</v>
       </c>
     </row>
     <row r="13" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A13" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B13" s="11">
-        <v>42863</v>
+        <v>42861</v>
       </c>
       <c r="C13" s="10">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D13" s="11">
         <v>42873</v>
@@ -1714,7 +1747,7 @@
     </row>
     <row r="14" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B14" s="11">
         <v>42874</v>
@@ -1728,7 +1761,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B15" s="6">
         <v>42856</v>
@@ -1752,10 +1785,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1870,7 +1903,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1893,7 +1926,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B8" s="4">
         <v>7.5</v>
@@ -1906,7 +1939,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1946,7 +1979,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="4">
-        <f>B12*C12</f>
+        <f t="shared" ref="D12:D17" si="1">B12*C12</f>
         <v>58</v>
       </c>
       <c r="E12" s="4" t="s">
@@ -1964,7 +1997,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="1">
-        <f>B13*C13</f>
+        <f t="shared" si="1"/>
         <v>17.66</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -1982,7 +2015,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="1">
-        <f>B14*C14</f>
+        <f t="shared" si="1"/>
         <v>12.95</v>
       </c>
       <c r="E14" s="2" t="s">
@@ -1991,7 +2024,7 @@
     </row>
     <row r="15" spans="1:5" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B15" s="4">
         <v>16.28</v>
@@ -2000,16 +2033,16 @@
         <v>1</v>
       </c>
       <c r="D15" s="4">
-        <f>B15*C15</f>
+        <f t="shared" si="1"/>
         <v>16.28</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B16" s="4">
         <v>5.9</v>
@@ -2018,10 +2051,28 @@
         <v>1</v>
       </c>
       <c r="D16" s="4">
-        <f>B16*C16</f>
+        <f t="shared" si="1"/>
         <v>5.9</v>
       </c>
       <c r="E16" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="1">
+        <v>26</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
All changes until March 07
- some new stl files added.
- updated proposal and excel file.
- remote and esc testing completed.
</commit_message>
<xml_diff>
--- a/Robotics.xlsx
+++ b/Robotics.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="460" windowWidth="25480" windowHeight="15540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="460" windowWidth="25480" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
   <si>
     <t>Todos</t>
   </si>
@@ -90,33 +90,12 @@
     <t>https://www.amazon.com/RioRand-A2212-1000KV-Outrunner-Quad-Rotor/dp/B00M3UONLM/ref=sr_1_2?ie=UTF8&amp;qid=1488501097&amp;sr=8-2&amp;keywords=4X+A2212+1000KV+Brushless+Motor</t>
   </si>
   <si>
-    <t>Bluefruit LE</t>
-  </si>
-  <si>
-    <t>https://www.adafruit.com/products/1697</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Adafruit-Barometric-Pressure-Temperature-Altitude/dp/B00JHJB2V6/ref=sr_1_1?ie=UTF8&amp;qid=1488504751&amp;sr=8-1&amp;keywords=barometer+arduino</t>
-  </si>
-  <si>
     <t>MPU 6050</t>
   </si>
   <si>
-    <t>BMP 180</t>
-  </si>
-  <si>
     <t>Design the frame</t>
   </si>
   <si>
-    <t>Assemble frame</t>
-  </si>
-  <si>
-    <t>Print frame</t>
-  </si>
-  <si>
-    <t>Electronics</t>
-  </si>
-  <si>
     <t>Test leveling and movement</t>
   </si>
   <si>
@@ -181,13 +160,22 @@
   </si>
   <si>
     <t>Test wireless control</t>
+  </si>
+  <si>
+    <t>Bluetooth Module</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Pass-Through-Communication-Compatible-Atomic-Market/dp/B00TNOO438/ref=sr_1_3?ie=UTF8&amp;qid=1488892564&amp;sr=8-3&amp;keywords=bluetooth+arduino</t>
+  </si>
+  <si>
+    <t>Wire electronics</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -240,11 +228,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF111111"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -282,20 +265,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -305,13 +291,12 @@
     <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="14" fontId="6" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="6" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="14">
     <cellStyle name="20% - Accent3" xfId="2" builtinId="38"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -321,6 +306,9 @@
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -383,46 +371,40 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$14</c:f>
+              <c:f>Sheet1!$A$2:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Design the frame</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Print frame</c:v>
+                  <c:v>Develop iOS Application</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Develop iOS Application</c:v>
+                  <c:v>Wire electronics</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Assemble frame</c:v>
+                  <c:v>Develop Wireless controlling</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Electronics</c:v>
+                  <c:v>Test wireless control</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Develop Wireless controlling</c:v>
+                  <c:v>Develop PID</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Test wireless control</c:v>
+                  <c:v>Test leveling and movement</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Develop PID</c:v>
+                  <c:v>Begin to reflect upon the project and schedule. </c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Test leveling and movement</c:v>
+                  <c:v>Implement GPS hardware</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Begin to reflect upon the project and schedule. </c:v>
+                  <c:v>Develop software for GPS</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Implement GPS hardware</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Develop software for GPS</c:v>
-                </c:pt>
-                <c:pt idx="12">
                   <c:v>Test final product</c:v>
                 </c:pt>
               </c:strCache>
@@ -430,10 +412,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$15</c:f>
+              <c:f>Sheet1!$B$2:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>42814.0</c:v>
                 </c:pt>
@@ -444,36 +426,30 @@
                   <c:v>42822.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42824.0</c:v>
+                  <c:v>42830.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42829.0</c:v>
+                  <c:v>42840.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>42835.0</c:v>
+                  <c:v>42844.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42841.0</c:v>
+                  <c:v>42853.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>42844.0</c:v>
+                  <c:v>42855.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>42849.0</c:v>
+                  <c:v>42856.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>42854.0</c:v>
+                  <c:v>42861.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>42856.0</c:v>
+                  <c:v>42874.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>42861.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>42874.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
                   <c:v>42856.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -495,46 +471,40 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$14</c:f>
+              <c:f>Sheet1!$A$2:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Design the frame</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Print frame</c:v>
+                  <c:v>Develop iOS Application</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Develop iOS Application</c:v>
+                  <c:v>Wire electronics</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Assemble frame</c:v>
+                  <c:v>Develop Wireless controlling</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Electronics</c:v>
+                  <c:v>Test wireless control</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Develop Wireless controlling</c:v>
+                  <c:v>Develop PID</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Test wireless control</c:v>
+                  <c:v>Test leveling and movement</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Develop PID</c:v>
+                  <c:v>Begin to reflect upon the project and schedule. </c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Test leveling and movement</c:v>
+                  <c:v>Implement GPS hardware</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Begin to reflect upon the project and schedule. </c:v>
+                  <c:v>Develop software for GPS</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Implement GPS hardware</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Develop software for GPS</c:v>
-                </c:pt>
-                <c:pt idx="12">
                   <c:v>Test final product</c:v>
                 </c:pt>
               </c:strCache>
@@ -542,50 +512,44 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$15</c:f>
+              <c:f>Sheet1!$C$2:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>5.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>14.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>5.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.0</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.0</c:v>
+                  <c:v>14.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.0</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>14.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
                   <c:v>25.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -602,11 +566,11 @@
         </c:dLbls>
         <c:gapWidth val="30"/>
         <c:overlap val="100"/>
-        <c:axId val="695017184"/>
-        <c:axId val="695031600"/>
+        <c:axId val="2041459168"/>
+        <c:axId val="2041461488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="695017184"/>
+        <c:axId val="2041459168"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -616,7 +580,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="695031600"/>
+        <c:crossAx val="2041461488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -624,7 +588,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="695031600"/>
+        <c:axId val="2041461488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="42885.0"/>
@@ -636,7 +600,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="695017184"/>
+        <c:crossAx val="2041459168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1235,7 +1199,7 @@
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>103482</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1521,10 +1485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView zoomScale="140" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1550,36 +1514,36 @@
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B2" s="6">
         <v>42814</v>
@@ -1593,188 +1557,160 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="B3" s="6">
         <v>42822</v>
       </c>
       <c r="C3" s="4">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D3" s="6">
-        <v>42796</v>
+        <v>42832</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B4" s="6">
         <v>42822</v>
       </c>
       <c r="C4" s="4">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D4" s="6">
-        <v>42832</v>
+        <v>42829</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="B5" s="6">
-        <v>42824</v>
+        <v>42830</v>
       </c>
       <c r="C5" s="4">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D5" s="6">
-        <v>42829</v>
+        <v>42840</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="B6" s="6">
-        <v>42829</v>
+        <v>42840</v>
       </c>
       <c r="C6" s="4">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D6" s="6">
-        <v>42832</v>
+        <v>42844</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="B7" s="6">
-        <v>42835</v>
+        <v>42844</v>
       </c>
       <c r="C7" s="4">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D7" s="6">
-        <v>42841</v>
+        <v>42854</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="B8" s="6">
-        <v>42841</v>
+        <v>42853</v>
       </c>
       <c r="C8" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D8" s="6">
-        <v>42844</v>
+        <v>42853</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B9" s="6">
-        <v>42844</v>
+        <v>42855</v>
       </c>
       <c r="C9" s="4">
+        <v>2</v>
+      </c>
+      <c r="D9" s="6">
+        <v>42859</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="12">
+        <v>42856</v>
+      </c>
+      <c r="C10" s="11">
+        <v>5</v>
+      </c>
+      <c r="D10" s="12">
+        <v>42860</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="10">
+        <v>42861</v>
+      </c>
+      <c r="C11" s="9">
+        <v>14</v>
+      </c>
+      <c r="D11" s="10">
+        <v>42873</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="10">
+        <v>42874</v>
+      </c>
+      <c r="C12" s="9">
         <v>7</v>
       </c>
-      <c r="D9" s="6">
-        <v>42848</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A10" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="6">
-        <v>42849</v>
-      </c>
-      <c r="C10" s="4">
-        <v>5</v>
-      </c>
-      <c r="D10" s="6">
-        <v>42853</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A11" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="6">
-        <v>42854</v>
-      </c>
-      <c r="C11" s="4">
-        <v>3</v>
-      </c>
-      <c r="D11" s="6">
-        <v>42859</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="13">
+      <c r="D12" s="10">
+        <v>42880</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="6">
         <v>42856</v>
       </c>
-      <c r="C12" s="12">
-        <v>5</v>
-      </c>
-      <c r="D12" s="13">
-        <v>42860</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="11">
-        <v>42861</v>
-      </c>
-      <c r="C13" s="10">
-        <v>14</v>
-      </c>
-      <c r="D13" s="11">
-        <v>42873</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="11">
-        <v>42874</v>
-      </c>
-      <c r="C14" s="10">
-        <v>7</v>
-      </c>
-      <c r="D14" s="11">
-        <v>42880</v>
+      <c r="C13" s="4">
+        <v>25</v>
+      </c>
+      <c r="D13" s="6">
+        <v>42875</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A15" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="6">
-        <v>42856</v>
-      </c>
-      <c r="C15" s="4">
-        <v>25</v>
-      </c>
-      <c r="D15" s="6">
-        <v>42875</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.15">
-      <c r="D17" s="5"/>
+      <c r="D15" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1785,18 +1721,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView zoomScale="137" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" style="9" customWidth="1"/>
-    <col min="2" max="3" width="10.83203125" style="9"/>
-    <col min="4" max="4" width="13" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="9"/>
+    <col min="1" max="1" width="13.83203125" style="8" customWidth="1"/>
+    <col min="2" max="3" width="10.83203125" style="8"/>
+    <col min="4" max="4" width="13" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -1824,11 +1760,11 @@
         <v>38.33</v>
       </c>
       <c r="C2" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="4">
-        <f t="shared" ref="D2:D7" si="0">B2*C2</f>
-        <v>38.33</v>
+        <f t="shared" ref="D2:D4" si="0">B2*C2</f>
+        <v>0</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>16</v>
@@ -1854,20 +1790,20 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B4" s="4">
-        <v>19.95</v>
+        <v>8.99</v>
       </c>
       <c r="C4" s="4">
         <v>1</v>
       </c>
       <c r="D4" s="4">
         <f t="shared" si="0"/>
-        <v>19.95</v>
+        <v>8.99</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1890,7 +1826,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B6" s="4">
         <v>6.94</v>
@@ -1903,57 +1839,48 @@
         <v>0</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
-        <v>24</v>
+      <c r="A7" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="B7" s="4">
-        <v>9.9499999999999993</v>
+        <v>7.5</v>
       </c>
       <c r="C7" s="4">
         <v>0</v>
       </c>
       <c r="D7" s="4">
-        <f t="shared" si="0"/>
+        <f>B7*C7</f>
         <v>0</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>22</v>
+      <c r="E7" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C8" s="4">
-        <v>0</v>
-      </c>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
       <c r="D8" s="4">
-        <f>B8*C8</f>
-        <v>0</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>41</v>
-      </c>
+        <f>D4+D6+D3+D2+D5</f>
+        <v>40.64</v>
+      </c>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4">
-        <f>D7+D4+D6+D3+D2+D5</f>
-        <v>89.929999999999993</v>
-      </c>
-      <c r="E9" s="4"/>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1961,127 +1888,119 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="B11" s="4">
+        <v>58</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1</v>
+      </c>
+      <c r="D11" s="4">
+        <f t="shared" ref="D11:D16" si="1">B11*C11</f>
+        <v>58</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="4">
-        <v>58</v>
-      </c>
-      <c r="C12" s="4">
+        <v>13</v>
+      </c>
+      <c r="B12" s="1">
+        <v>17.66</v>
+      </c>
+      <c r="C12" s="1">
         <v>1</v>
       </c>
-      <c r="D12" s="4">
-        <f t="shared" ref="D12:D17" si="1">B12*C12</f>
-        <v>58</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>19</v>
+      <c r="D12" s="1">
+        <f t="shared" si="1"/>
+        <v>17.66</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B13" s="1">
-        <v>17.66</v>
+        <v>12.95</v>
       </c>
       <c r="C13" s="1">
         <v>1</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="1"/>
-        <v>17.66</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="1">
         <v>12.95</v>
       </c>
-      <c r="C14" s="1">
+      <c r="E13" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="4">
+        <v>16.28</v>
+      </c>
+      <c r="C14" s="4">
         <v>1</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="4">
         <f t="shared" si="1"/>
-        <v>12.95</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>12</v>
+        <v>16.28</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B15" s="4">
-        <v>16.28</v>
+        <v>5.9</v>
       </c>
       <c r="C15" s="4">
         <v>1</v>
       </c>
       <c r="D15" s="4">
         <f t="shared" si="1"/>
-        <v>16.28</v>
+        <v>5.9</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A16" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="4">
-        <v>5.9</v>
-      </c>
-      <c r="C16" s="4">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="1">
+        <v>26</v>
+      </c>
+      <c r="C16" s="1">
         <v>1</v>
       </c>
-      <c r="D16" s="4">
-        <f t="shared" si="1"/>
-        <v>5.9</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" s="1">
-        <v>26</v>
-      </c>
-      <c r="C17" s="1">
-        <v>1</v>
-      </c>
-      <c r="D17" s="1">
+      <c r="D16" s="1">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>47</v>
+      <c r="E16" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E14" r:id="rId1"/>
+    <hyperlink ref="E13" r:id="rId1"/>
     <hyperlink ref="E2" r:id="rId2"/>
-    <hyperlink ref="E8" r:id="rId3"/>
+    <hyperlink ref="E7" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes until April 7
- iOS remote bluetooth classes added
- stick movement added.
- ESC_simple code verified.
</commit_message>
<xml_diff>
--- a/Robotics.xlsx
+++ b/Robotics.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
   <si>
     <t>Todos</t>
   </si>
@@ -60,9 +60,6 @@
     <t>LiPo Battery </t>
   </si>
   <si>
-    <t>https://www.amazon.com/Gens-ace-Battery-2200mAh-Airplane/dp/B00WJN4LG0/ref=sr_1_3?ie=UTF8&amp;qid=1488499661&amp;sr=8-3&amp;keywords=lipo+battery+11.1v</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -90,12 +87,6 @@
     <t>https://www.amazon.com/RioRand-A2212-1000KV-Outrunner-Quad-Rotor/dp/B00M3UONLM/ref=sr_1_2?ie=UTF8&amp;qid=1488501097&amp;sr=8-2&amp;keywords=4X+A2212+1000KV+Brushless+Motor</t>
   </si>
   <si>
-    <t>MPU 6050</t>
-  </si>
-  <si>
-    <t>Design the frame</t>
-  </si>
-  <si>
     <t>Test leveling and movement</t>
   </si>
   <si>
@@ -126,15 +117,6 @@
     <t>Test final product</t>
   </si>
   <si>
-    <t>https://www.amazon.com/Kootek-MPU-6050-MPU6050-sensors-Accelerometer/dp/B008BOPN40/ref=sr_1_4?ie=UTF8&amp;qid=1488655663&amp;sr=8-4&amp;keywords=mpu+6050</t>
-  </si>
-  <si>
-    <t>Wood Screw 34mm, 19mm, 12mm * 3mm 6g A2 Stainless Steel</t>
-  </si>
-  <si>
-    <t>http://www.ebay.com/itm/3mm-6g-A2-STAINLESS-STEEL-WOOD-SCREWS-POZI-CSK-10mm-THROUGH-TO-50mm-/190718538596?var=&amp;hash=item2c67b5f364:m:mWmH-3MwpEqMHxtEfEkZxsw</t>
-  </si>
-  <si>
     <t>Folding props</t>
   </si>
   <si>
@@ -169,13 +151,16 @@
   </si>
   <si>
     <t>Wire electronics</t>
+  </si>
+  <si>
+    <t>https://goo.gl/0CS44u</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -210,20 +195,8 @@
       <name val="Times Roman"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Times Roman"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Times New Roman"/>
     </font>
     <font>
@@ -265,38 +238,37 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="14">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="14" fontId="6" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="6" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="14">
+  <cellStyles count="15">
     <cellStyle name="20% - Accent3" xfId="2" builtinId="38"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -309,6 +281,7 @@
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -371,40 +344,37 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$12</c:f>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>Design the frame</c:v>
+                  <c:v>Develop iOS Application</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Develop iOS Application</c:v>
+                  <c:v>Wire electronics</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Wire electronics</c:v>
+                  <c:v>Develop Wireless controlling</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Develop Wireless controlling</c:v>
+                  <c:v>Test wireless control</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Test wireless control</c:v>
+                  <c:v>Develop PID</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Develop PID</c:v>
+                  <c:v>Test leveling and movement</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Test leveling and movement</c:v>
+                  <c:v>Begin to reflect upon the project and schedule. </c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Begin to reflect upon the project and schedule. </c:v>
+                  <c:v>Implement GPS hardware</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Implement GPS hardware</c:v>
+                  <c:v>Develop software for GPS</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Develop software for GPS</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>Test final product</c:v>
                 </c:pt>
               </c:strCache>
@@ -412,44 +382,41 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$13</c:f>
+              <c:f>Sheet1!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>42814.0</c:v>
+                  <c:v>42822.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>42822.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42822.0</c:v>
+                  <c:v>42830.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42830.0</c:v>
+                  <c:v>42840.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42840.0</c:v>
+                  <c:v>42844.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>42844.0</c:v>
+                  <c:v>42853.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42853.0</c:v>
+                  <c:v>42856.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>42855.0</c:v>
+                  <c:v>42857.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>42856.0</c:v>
+                  <c:v>42860.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>42861.0</c:v>
+                  <c:v>42874.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>42874.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
                   <c:v>42856.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -471,40 +438,37 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$12</c:f>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>Design the frame</c:v>
+                  <c:v>Develop iOS Application</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Develop iOS Application</c:v>
+                  <c:v>Wire electronics</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Wire electronics</c:v>
+                  <c:v>Develop Wireless controlling</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Develop Wireless controlling</c:v>
+                  <c:v>Test wireless control</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Test wireless control</c:v>
+                  <c:v>Develop PID</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Develop PID</c:v>
+                  <c:v>Test leveling and movement</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Test leveling and movement</c:v>
+                  <c:v>Begin to reflect upon the project and schedule. </c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Begin to reflect upon the project and schedule. </c:v>
+                  <c:v>Implement GPS hardware</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Implement GPS hardware</c:v>
+                  <c:v>Develop software for GPS</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Develop software for GPS</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>Test final product</c:v>
                 </c:pt>
               </c:strCache>
@@ -512,44 +476,41 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$13</c:f>
+              <c:f>Sheet1!$C$2:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>8.0</c:v>
+                  <c:v>14.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>14.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="9">
                   <c:v>7.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>14.0</c:v>
-                </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
                   <c:v>25.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -566,11 +527,11 @@
         </c:dLbls>
         <c:gapWidth val="30"/>
         <c:overlap val="100"/>
-        <c:axId val="2041459168"/>
-        <c:axId val="2041461488"/>
+        <c:axId val="-2048564960"/>
+        <c:axId val="-2048369984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2041459168"/>
+        <c:axId val="-2048564960"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -580,7 +541,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2041461488"/>
+        <c:crossAx val="-2048369984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -588,7 +549,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2041461488"/>
+        <c:axId val="-2048369984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="42885.0"/>
@@ -600,7 +561,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2041459168"/>
+        <c:crossAx val="-2048564960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1191,16 +1152,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>18814</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>172357</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>136878</xdr:rowOff>
+      <xdr:rowOff>136879</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>103482</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>825500</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>72572</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1485,232 +1446,215 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="10.5" style="4" customWidth="1"/>
-    <col min="4" max="4" width="13" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="4"/>
+    <col min="1" max="1" width="17.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="13" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="5">
+        <v>42822</v>
+      </c>
+      <c r="C2" s="3">
+        <v>14</v>
+      </c>
+      <c r="D2" s="5">
+        <v>42832</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="5">
+        <v>42822</v>
+      </c>
+      <c r="C3" s="3">
+        <v>7</v>
+      </c>
+      <c r="D3" s="5">
+        <v>42829</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="5">
+        <v>42830</v>
+      </c>
+      <c r="C4" s="3">
+        <v>10</v>
+      </c>
+      <c r="D4" s="5">
+        <v>42840</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="5">
+        <v>42840</v>
+      </c>
+      <c r="C5" s="3">
+        <v>5</v>
+      </c>
+      <c r="D5" s="5">
+        <v>42844</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="B6" s="5">
+        <v>42844</v>
+      </c>
+      <c r="C6" s="3">
+        <v>10</v>
+      </c>
+      <c r="D6" s="5">
+        <v>42854</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="5">
+        <v>42853</v>
+      </c>
+      <c r="C7" s="3">
+        <v>5</v>
+      </c>
+      <c r="D7" s="5">
+        <v>42853</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="5">
+        <v>42856</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2</v>
+      </c>
+      <c r="D8" s="5">
+        <v>42857</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="10">
+        <v>42857</v>
+      </c>
+      <c r="C9" s="9">
+        <v>3</v>
+      </c>
+      <c r="D9" s="10">
+        <v>42859</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="8">
+        <v>42860</v>
+      </c>
+      <c r="C10" s="7">
+        <v>14</v>
+      </c>
+      <c r="D10" s="8">
+        <v>42873</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="8">
+        <v>42874</v>
+      </c>
+      <c r="C11" s="7">
+        <v>7</v>
+      </c>
+      <c r="D11" s="8">
+        <v>42880</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="5">
+        <v>42856</v>
+      </c>
+      <c r="C12" s="3">
         <v>25</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="6">
-        <v>42814</v>
-      </c>
-      <c r="C2" s="4">
-        <v>8</v>
-      </c>
-      <c r="D2" s="6">
-        <v>42821</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A3" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="6">
-        <v>42822</v>
-      </c>
-      <c r="C3" s="4">
-        <v>14</v>
-      </c>
-      <c r="D3" s="6">
-        <v>42832</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A4" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="6">
-        <v>42822</v>
-      </c>
-      <c r="C4" s="4">
-        <v>7</v>
-      </c>
-      <c r="D4" s="6">
-        <v>42829</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A5" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="6">
-        <v>42830</v>
-      </c>
-      <c r="C5" s="4">
-        <v>10</v>
-      </c>
-      <c r="D5" s="6">
-        <v>42840</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A6" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="6">
-        <v>42840</v>
-      </c>
-      <c r="C6" s="4">
-        <v>5</v>
-      </c>
-      <c r="D6" s="6">
-        <v>42844</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="6">
-        <v>42844</v>
-      </c>
-      <c r="C7" s="4">
-        <v>10</v>
-      </c>
-      <c r="D7" s="6">
-        <v>42854</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="6">
-        <v>42853</v>
-      </c>
-      <c r="C8" s="4">
-        <v>5</v>
-      </c>
-      <c r="D8" s="6">
-        <v>42853</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="6">
-        <v>42855</v>
-      </c>
-      <c r="C9" s="4">
-        <v>2</v>
-      </c>
-      <c r="D9" s="6">
-        <v>42859</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="12">
-        <v>42856</v>
-      </c>
-      <c r="C10" s="11">
-        <v>5</v>
-      </c>
-      <c r="D10" s="12">
-        <v>42860</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="10">
-        <v>42861</v>
-      </c>
-      <c r="C11" s="9">
-        <v>14</v>
-      </c>
-      <c r="D11" s="10">
-        <v>42873</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="10">
-        <v>42874</v>
-      </c>
-      <c r="C12" s="9">
-        <v>7</v>
-      </c>
-      <c r="D12" s="10">
-        <v>42880</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="6">
-        <v>42856</v>
-      </c>
-      <c r="C13" s="4">
-        <v>25</v>
-      </c>
-      <c r="D13" s="6">
+      <c r="D12" s="5">
         <v>42875</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="D15" s="5"/>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="D14" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1721,284 +1665,228 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView zoomScale="137" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E5"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" style="8" customWidth="1"/>
-    <col min="2" max="3" width="10.83203125" style="8"/>
-    <col min="4" max="4" width="13" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="8"/>
+    <col min="1" max="1" width="13.83203125" style="6" customWidth="1"/>
+    <col min="2" max="3" width="10.83203125" style="6"/>
+    <col min="4" max="4" width="13" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="4">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1">
         <v>38.33</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="1">
         <v>0</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="1">
         <f t="shared" ref="D2:D4" si="0">B2*C2</f>
         <v>0</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>16</v>
+      <c r="E2" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="1">
         <v>13.99</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="1">
         <v>1</v>
       </c>
-      <c r="D3" s="4">
-        <f t="shared" si="0"/>
-        <v>13.99</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>10</v>
+      <c r="D3" s="1">
+        <v>18.64</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="4">
+      <c r="A4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="1">
         <v>8.99</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="1">
         <v>1</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="1">
         <f t="shared" si="0"/>
         <v>8.99</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>45</v>
+      <c r="E4" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="4">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1">
         <v>17.66</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="1">
         <v>1</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="1">
         <f>B5*C5</f>
         <v>17.66</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>14</v>
+      <c r="E5" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="4">
-        <v>6.94</v>
-      </c>
-      <c r="C6" s="4">
-        <v>0</v>
-      </c>
-      <c r="D6" s="4">
-        <f>B6*C6</f>
-        <v>0</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>32</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1">
+        <f>D3+D4+D5</f>
+        <v>45.290000000000006</v>
+      </c>
+      <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="C7" s="4">
-        <v>0</v>
-      </c>
-      <c r="D7" s="4">
-        <f>B7*C7</f>
-        <v>0</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>34</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4">
-        <f>D4+D6+D3+D2+D5</f>
-        <v>40.64</v>
-      </c>
-      <c r="E8" s="4"/>
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="3">
+        <v>58</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" ref="D9:D13" si="1">B9*C9</f>
+        <v>58</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="4">
-        <v>58</v>
-      </c>
-      <c r="C11" s="4">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1">
+        <v>12.95</v>
+      </c>
+      <c r="C10" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="4">
-        <f t="shared" ref="D11:D16" si="1">B11*C11</f>
-        <v>58</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="1">
-        <v>17.66</v>
-      </c>
-      <c r="C12" s="1">
+      <c r="D10" s="1">
+        <f t="shared" si="1"/>
+        <v>12.95</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="3">
+        <v>16.28</v>
+      </c>
+      <c r="C11" s="3">
         <v>1</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D11" s="3">
         <f t="shared" si="1"/>
-        <v>17.66</v>
+        <v>16.28</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="3">
+        <v>5.9</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="1"/>
+        <v>5.9</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="B13" s="1">
-        <v>12.95</v>
+        <v>26</v>
       </c>
       <c r="C13" s="1">
         <v>1</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="1"/>
-        <v>12.95</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A14" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="4">
-        <v>16.28</v>
-      </c>
-      <c r="C14" s="4">
-        <v>1</v>
-      </c>
-      <c r="D14" s="4">
-        <f t="shared" si="1"/>
-        <v>16.28</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A15" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="4">
-        <v>5.9</v>
-      </c>
-      <c r="C15" s="4">
-        <v>1</v>
-      </c>
-      <c r="D15" s="4">
-        <f t="shared" si="1"/>
-        <v>5.9</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="1">
         <v>26</v>
       </c>
-      <c r="C16" s="1">
-        <v>1</v>
-      </c>
-      <c r="D16" s="1">
-        <f t="shared" si="1"/>
-        <v>26</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>40</v>
+      <c r="E13" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E13" r:id="rId1"/>
+    <hyperlink ref="E10" r:id="rId1"/>
     <hyperlink ref="E2" r:id="rId2"/>
-    <hyperlink ref="E7" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>